<commit_message>
1st commit by VG
</commit_message>
<xml_diff>
--- a/TestData/MyWorkshop.xlsx
+++ b/TestData/MyWorkshop.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinay\Gitlab projects\SeleniumDataDrivenV1\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13653B1B-575E-4894-AAA4-865768F773D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D4187D-D044-4804-88AB-1DDA55846306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -119,19 +119,19 @@
     <t>Arpit Agarwal</t>
   </si>
   <si>
-    <t>abcx16@gmail.com</t>
-  </si>
-  <si>
-    <t>abcx17@gmail.com</t>
-  </si>
-  <si>
-    <t>abcx18@gmail.com</t>
-  </si>
-  <si>
-    <t>abcx19@gmail.com</t>
-  </si>
-  <si>
     <t>Vinay Guptaa</t>
+  </si>
+  <si>
+    <t>abcx22@gmail.com</t>
+  </si>
+  <si>
+    <t>abcx23@gmail.com</t>
+  </si>
+  <si>
+    <t>abcx24@gmail.com</t>
+  </si>
+  <si>
+    <t>abcx26@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -499,7 +499,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -524,18 +524,18 @@
     </row>
     <row r="2" spans="1:3" ht="23.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="23.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -546,7 +546,7 @@
     </row>
     <row r="4" spans="1:3" ht="23.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
@@ -557,7 +557,7 @@
     </row>
     <row r="5" spans="1:3" ht="23.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
@@ -569,10 +569,10 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{62ECA280-E0E9-4FF3-96C5-E9B3A3536F87}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{8A8DBD28-8186-4C99-9380-D173675D694A}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{0C49A05C-5302-4891-96EE-2E91D0AE7A0B}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{DBDC0186-335F-46DA-A7A8-B5DCB7F02A58}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{78151AA6-6019-49DD-B290-9940198B0D69}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{1A554763-A9DE-4858-B2EC-B1F44F691D9D}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{15726643-DE2E-4751-8B74-9947208DD46E}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{01D9648A-6479-4AB5-B592-3DEB70C8547F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
@@ -584,7 +584,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -627,7 +627,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
@@ -653,7 +653,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
@@ -679,7 +679,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -705,7 +705,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>

</xml_diff>